<commit_message>
Add customer inquiry category classification and unit tests
</commit_message>
<xml_diff>
--- a/src/RouteCustomerInquiry/Tests/TestData/ClassifyCustomerInquiry.xlsx
+++ b/src/RouteCustomerInquiry/Tests/TestData/ClassifyCustomerInquiry.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="22">
   <si>
     <t>Neutral</t>
   </si>
@@ -68,6 +68,18 @@
   </si>
   <si>
     <t>Hi, how do I check if the item I ordered was already shipped. Can you help please?</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Already handled, just venting. It was a pretty big bummer.</t>
+  </si>
+  <si>
+    <t>Thanks for quick response. Pic attached.</t>
+  </si>
+  <si>
+    <t>Pls call me on 9820255387</t>
   </si>
 </sst>
 </file>
@@ -138,7 +150,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
@@ -158,6 +170,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -462,7 +475,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -523,69 +536,102 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
         <v>17</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>16</v>
+      <c r="A8" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>13</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>